<commit_message>
Changed the Pit Scouting Sheet a Bit
</commit_message>
<xml_diff>
--- a/Pre-Season/Sheet Revisions/2019 Pit Scouting Sheet Modified.xlsx
+++ b/Pre-Season/Sheet Revisions/2019 Pit Scouting Sheet Modified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\team3641\2019\Scouting Laptop Github\2019Scouting\Pre-Season\Sheet Revisions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EE306C-11A3-4916-AB0C-29021DA72899}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB7E34D-2963-4B95-8523-18593F58039C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,7 +590,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -913,7 +913,7 @@
       <c r="A31" s="10"/>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" gridLines="1"/>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="65" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
 </worksheet>

</xml_diff>